<commit_message>
libro de clases funcionando
</commit_message>
<xml_diff>
--- a/Backend/assets/excelAttendance/9AtWGv0z3lCdpKo5U9DI.xlsx
+++ b/Backend/assets/excelAttendance/9AtWGv0z3lCdpKo5U9DI.xlsx
@@ -1,12 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="3045" yWindow="1845" windowWidth="21600" windowHeight="11385" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -412,7 +412,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
@@ -430,6 +430,21 @@
       <c r="D1" t="n">
         <v>8</v>
       </c>
+      <c r="E1" t="n">
+        <v>11</v>
+      </c>
+      <c r="F1" t="n">
+        <v>12</v>
+      </c>
+      <c r="G1" t="n">
+        <v>13</v>
+      </c>
+      <c r="H1" t="n">
+        <v>14</v>
+      </c>
+      <c r="I1" t="n">
+        <v>15</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -437,6 +452,36 @@
       </c>
       <c r="B2" t="n">
         <v>2</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>